<commit_message>
unlocked all the row for unlimited entries
</commit_message>
<xml_diff>
--- a/data/Output_SunMusic.xlsx
+++ b/data/Output_SunMusic.xlsx
@@ -75,12 +75,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -616,7 +617,7 @@
       <c r="BH1" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="BI1" s="2" t="n"/>
+      <c r="BI1" s="3" t="n"/>
     </row>
     <row r="2" ht="21" customHeight="1">
       <c r="O2" s="1" t="inlineStr">
@@ -849,16 +850,16 @@
           <t>MAGNUM PELE_PISTA  IN APR'25</t>
         </is>
       </c>
-      <c r="BI2" s="2" t="n"/>
+      <c r="BI2" s="3" t="n"/>
     </row>
     <row r="3" ht="21" customHeight="1">
-      <c r="K3" s="3" t="inlineStr">
+      <c r="K3" s="4" t="inlineStr">
         <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="L3" s="4" t="n"/>
-      <c r="M3" s="3" t="inlineStr">
+      <c r="L3" s="5" t="n"/>
+      <c r="M3" s="4" t="inlineStr">
         <is>
           <t>MAX</t>
         </is>
@@ -1093,15 +1094,15 @@
           <t>MAG PELEPISTA 30S 2025 HUL TLF</t>
         </is>
       </c>
-      <c r="BI3" s="2" t="n"/>
+      <c r="BI3" s="3" t="n"/>
     </row>
     <row r="4" ht="21" customHeight="1">
-      <c r="K4" s="3">
+      <c r="K4" s="4">
         <f>ROUND(MIN($P$4:$BI$4), 0)</f>
         <v/>
       </c>
-      <c r="L4" s="4" t="n"/>
-      <c r="M4" s="3">
+      <c r="L4" s="5" t="n"/>
+      <c r="M4" s="4">
         <f>ROUND(MAX($P$4:$BI$4), 0)</f>
         <v/>
       </c>
@@ -1245,21 +1246,21 @@
       <c r="BH4" s="2" t="n">
         <v>6300</v>
       </c>
-      <c r="BI4" s="2" t="n">
+      <c r="BI4" s="3" t="n">
         <v>181552</v>
       </c>
-      <c r="BJ4" s="5">
-        <f>ROUND(SUM(P4:BI4), 0)</f>
+      <c r="BJ4" s="6">
+        <f>ROUND(SUM(P4:BH4), 0)</f>
         <v/>
       </c>
     </row>
     <row r="5" ht="21" customHeight="1">
-      <c r="K5" s="3">
+      <c r="K5" s="4">
         <f>MIN($P$5:$BI$5)</f>
         <v/>
       </c>
-      <c r="L5" s="4" t="n"/>
-      <c r="M5" s="3">
+      <c r="L5" s="5" t="n"/>
+      <c r="M5" s="4">
         <f>MAX($P$5:$BI$5)</f>
         <v/>
       </c>
@@ -1403,21 +1404,21 @@
       <c r="BH5" s="2" t="n">
         <v>3.9375</v>
       </c>
-      <c r="BI5" s="2" t="n">
+      <c r="BI5" s="3" t="n">
         <v>113.4703125</v>
       </c>
-      <c r="BJ5" s="5">
-        <f>ROUND(SUM(P5:BI5), 0)</f>
+      <c r="BJ5" s="6">
+        <f>ROUND(SUM(P5:BH5), 0)</f>
         <v/>
       </c>
     </row>
     <row r="6" ht="21" customHeight="1">
-      <c r="K6" s="3">
+      <c r="K6" s="4">
         <f>MIN($P$6:$BI$6)</f>
         <v/>
       </c>
-      <c r="L6" s="4" t="n"/>
-      <c r="M6" s="3">
+      <c r="L6" s="5" t="n"/>
+      <c r="M6" s="4">
         <f>MAX($P$6:$BI$6)</f>
         <v/>
       </c>
@@ -1606,7 +1607,6 @@
         <f>IFERROR((SUMPRODUCT(($O$24:$O$34=$O6)*($E$24:$E$34)*(BH$1/10)*(BH$24:BH$34))/BH10), 0)</f>
         <v/>
       </c>
-      <c r="BI6" s="6" t="n"/>
     </row>
     <row r="7" ht="21" customHeight="1">
       <c r="O7" s="1" t="inlineStr">
@@ -1794,7 +1794,6 @@
         <f>IFERROR(SUMPRODUCT(($O$24:$O$34=$O7)*($E$24:$E$34)*(BH$1/10)*(BH$24:BH$34)), 0)</f>
         <v/>
       </c>
-      <c r="BI7" s="6" t="n"/>
     </row>
     <row r="8" ht="21" customHeight="1">
       <c r="O8" s="1" t="inlineStr">
@@ -1802,70 +1801,69 @@
           <t>IB ID</t>
         </is>
       </c>
-      <c r="P8" s="6" t="n"/>
-      <c r="Q8" s="6" t="n"/>
-      <c r="R8" s="6" t="n"/>
-      <c r="S8" s="6" t="n"/>
-      <c r="T8" s="6" t="n"/>
-      <c r="U8" s="6" t="n"/>
-      <c r="V8" s="6" t="n"/>
-      <c r="W8" s="6" t="n"/>
-      <c r="X8" s="6" t="n"/>
-      <c r="Y8" s="6" t="n"/>
-      <c r="Z8" s="6" t="n"/>
-      <c r="AA8" s="6" t="n"/>
-      <c r="AB8" s="6" t="n"/>
-      <c r="AC8" s="6" t="n"/>
-      <c r="AD8" s="6" t="n"/>
-      <c r="AE8" s="6" t="n"/>
-      <c r="AF8" s="6" t="n"/>
-      <c r="AG8" s="6" t="n"/>
-      <c r="AH8" s="6" t="n"/>
-      <c r="AI8" s="6" t="n"/>
-      <c r="AJ8" s="6" t="n"/>
-      <c r="AK8" s="6" t="n"/>
-      <c r="AL8" s="6" t="n"/>
-      <c r="AM8" s="6" t="n"/>
-      <c r="AN8" s="6" t="n"/>
-      <c r="AO8" s="6" t="n"/>
-      <c r="AP8" s="6" t="n"/>
-      <c r="AQ8" s="6" t="n"/>
-      <c r="AR8" s="6" t="n"/>
-      <c r="AS8" s="6" t="n"/>
-      <c r="AT8" s="6" t="n"/>
-      <c r="AU8" s="6" t="n"/>
-      <c r="AV8" s="6" t="n"/>
-      <c r="AW8" s="6" t="n"/>
-      <c r="AX8" s="6" t="n"/>
-      <c r="AY8" s="6" t="n"/>
-      <c r="AZ8" s="6" t="n"/>
-      <c r="BA8" s="6" t="n"/>
-      <c r="BB8" s="6" t="n"/>
-      <c r="BC8" s="6" t="n"/>
-      <c r="BD8" s="6" t="n"/>
-      <c r="BE8" s="6" t="n"/>
-      <c r="BF8" s="6" t="n"/>
-      <c r="BG8" s="6" t="n"/>
-      <c r="BH8" s="6" t="n"/>
-      <c r="BI8" s="6" t="n"/>
+      <c r="P8" s="7" t="n"/>
+      <c r="Q8" s="7" t="n"/>
+      <c r="R8" s="7" t="n"/>
+      <c r="S8" s="7" t="n"/>
+      <c r="T8" s="7" t="n"/>
+      <c r="U8" s="7" t="n"/>
+      <c r="V8" s="7" t="n"/>
+      <c r="W8" s="7" t="n"/>
+      <c r="X8" s="7" t="n"/>
+      <c r="Y8" s="7" t="n"/>
+      <c r="Z8" s="7" t="n"/>
+      <c r="AA8" s="7" t="n"/>
+      <c r="AB8" s="7" t="n"/>
+      <c r="AC8" s="7" t="n"/>
+      <c r="AD8" s="7" t="n"/>
+      <c r="AE8" s="7" t="n"/>
+      <c r="AF8" s="7" t="n"/>
+      <c r="AG8" s="7" t="n"/>
+      <c r="AH8" s="7" t="n"/>
+      <c r="AI8" s="7" t="n"/>
+      <c r="AJ8" s="7" t="n"/>
+      <c r="AK8" s="7" t="n"/>
+      <c r="AL8" s="7" t="n"/>
+      <c r="AM8" s="7" t="n"/>
+      <c r="AN8" s="7" t="n"/>
+      <c r="AO8" s="7" t="n"/>
+      <c r="AP8" s="7" t="n"/>
+      <c r="AQ8" s="7" t="n"/>
+      <c r="AR8" s="7" t="n"/>
+      <c r="AS8" s="7" t="n"/>
+      <c r="AT8" s="7" t="n"/>
+      <c r="AU8" s="7" t="n"/>
+      <c r="AV8" s="7" t="n"/>
+      <c r="AW8" s="7" t="n"/>
+      <c r="AX8" s="7" t="n"/>
+      <c r="AY8" s="7" t="n"/>
+      <c r="AZ8" s="7" t="n"/>
+      <c r="BA8" s="7" t="n"/>
+      <c r="BB8" s="7" t="n"/>
+      <c r="BC8" s="7" t="n"/>
+      <c r="BD8" s="7" t="n"/>
+      <c r="BE8" s="7" t="n"/>
+      <c r="BF8" s="7" t="n"/>
+      <c r="BG8" s="7" t="n"/>
+      <c r="BH8" s="7" t="n"/>
     </row>
     <row r="9" ht="21" customHeight="1">
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="4" t="inlineStr">
         <is>
           <t>FCT LEFT</t>
         </is>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <f>SUM(N20:N9530)</f>
         <v/>
       </c>
-      <c r="D9" s="8" t="n"/>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="D9" s="9" t="n"/>
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>Pristine</t>
         </is>
       </c>
-      <c r="O9" s="9" t="inlineStr">
+      <c r="O9" s="10" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
@@ -2050,43 +2048,39 @@
         <f>ROUND(SUMPRODUCT(BH24:BH9530,$F$24:$F$9530)*BH$1/10, 0)</f>
         <v/>
       </c>
-      <c r="BI9" s="2">
-        <f>ROUND(SUMPRODUCT(BI24:BI9530,$F$24:$F$9530)*BI$1/10, 0)</f>
-        <v/>
-      </c>
-      <c r="BJ9" s="5">
-        <f>ROUND(SUM(P9:BI9), 0)</f>
+      <c r="BJ9" s="6">
+        <f>ROUND(SUM(P9:BH9), 0)</f>
         <v/>
       </c>
     </row>
     <row r="10" ht="21" customHeight="1">
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>%Allocation</t>
         </is>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <f>ROUND((BJ18/BJ5)*100, 0)</f>
         <v/>
       </c>
-      <c r="D10" s="8" t="n"/>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="D10" s="9" t="n"/>
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="K10" s="3" t="inlineStr">
+      <c r="K10" s="4" t="inlineStr">
         <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="L10" s="4" t="n"/>
-      <c r="M10" s="3" t="inlineStr">
+      <c r="L10" s="5" t="n"/>
+      <c r="M10" s="4" t="inlineStr">
         <is>
           <t>MAX</t>
         </is>
       </c>
-      <c r="O10" s="9" t="inlineStr">
+      <c r="O10" s="10" t="inlineStr">
         <is>
           <t>Allocated GRP</t>
         </is>
@@ -2271,41 +2265,37 @@
         <f>ROUND(SUMPRODUCT(BH24:BH9530,$E$24:$E$9530)*BH$1/10, 0)</f>
         <v/>
       </c>
-      <c r="BI10" s="2">
-        <f>ROUND(SUMPRODUCT(BI24:BI9530,$E$24:$E$9530)*BI$1/10, 0)</f>
-        <v/>
-      </c>
-      <c r="BJ10" s="5">
-        <f>ROUND(SUM(P10:BI10), 0)</f>
+      <c r="BJ10" s="6">
+        <f>ROUND(SUM(P10:BH10), 0)</f>
         <v/>
       </c>
     </row>
     <row r="11" ht="21" customHeight="1">
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="4" t="inlineStr">
         <is>
           <t>CPRP</t>
         </is>
       </c>
-      <c r="C11" s="7">
-        <f>(BK18/BJ18)*100000</f>
-        <v/>
-      </c>
-      <c r="D11" s="8" t="n"/>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="C11" s="8">
+        <f>SUM(BJ24:BJ55)</f>
+        <v/>
+      </c>
+      <c r="D11" s="9" t="n"/>
+      <c r="E11" s="4" t="inlineStr">
         <is>
           <t>CL.CPRP</t>
         </is>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="4">
         <f>MIN($P$11:$BI$11)</f>
         <v/>
       </c>
-      <c r="L11" s="4" t="n"/>
-      <c r="M11" s="3">
+      <c r="L11" s="5" t="n"/>
+      <c r="M11" s="4">
         <f>MAX($P$11:$BI$11)</f>
         <v/>
       </c>
-      <c r="O11" s="9" t="inlineStr">
+      <c r="O11" s="10" t="inlineStr">
         <is>
           <t>CPRP</t>
         </is>
@@ -2490,222 +2480,214 @@
         <f>IFERROR(ROUND(BH9/BH10, 0), 0)</f>
         <v/>
       </c>
-      <c r="BI11" s="2">
-        <f>IFERROR(ROUND(BI9/BI10, 0), 0)</f>
-        <v/>
-      </c>
     </row>
     <row r="12" ht="21" customHeight="1">
-      <c r="K12" s="3">
+      <c r="K12" s="4">
         <f>MIN($P$12:$BI$12)</f>
         <v/>
       </c>
-      <c r="L12" s="4" t="n"/>
-      <c r="M12" s="3">
+      <c r="L12" s="5" t="n"/>
+      <c r="M12" s="4">
         <f>MAX($P$12:$BI$12)</f>
         <v/>
       </c>
-      <c r="O12" s="9" t="inlineStr">
+      <c r="O12" s="10" t="inlineStr">
         <is>
           <t>GRP Allocation %</t>
         </is>
       </c>
-      <c r="P12" s="10">
+      <c r="P12" s="11">
         <f>IFERROR(ROUND(P10/P5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="Q12" s="10">
+      <c r="Q12" s="11">
         <f>IFERROR(ROUND(Q10/Q5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="11">
         <f>IFERROR(ROUND(R10/R5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="S12" s="10">
+      <c r="S12" s="11">
         <f>IFERROR(ROUND(S10/S5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="T12" s="10">
+      <c r="T12" s="11">
         <f>IFERROR(ROUND(T10/T5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="U12" s="10">
+      <c r="U12" s="11">
         <f>IFERROR(ROUND(U10/U5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="V12" s="10">
+      <c r="V12" s="11">
         <f>IFERROR(ROUND(V10/V5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="W12" s="10">
+      <c r="W12" s="11">
         <f>IFERROR(ROUND(W10/W5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="X12" s="10">
+      <c r="X12" s="11">
         <f>IFERROR(ROUND(X10/X5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="Y12" s="10">
+      <c r="Y12" s="11">
         <f>IFERROR(ROUND(Y10/Y5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="Z12" s="10">
+      <c r="Z12" s="11">
         <f>IFERROR(ROUND(Z10/Z5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AA12" s="10">
+      <c r="AA12" s="11">
         <f>IFERROR(ROUND(AA10/AA5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AB12" s="10">
+      <c r="AB12" s="11">
         <f>IFERROR(ROUND(AB10/AB5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AC12" s="10">
+      <c r="AC12" s="11">
         <f>IFERROR(ROUND(AC10/AC5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AD12" s="10">
+      <c r="AD12" s="11">
         <f>IFERROR(ROUND(AD10/AD5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AE12" s="10">
+      <c r="AE12" s="11">
         <f>IFERROR(ROUND(AE10/AE5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AF12" s="10">
+      <c r="AF12" s="11">
         <f>IFERROR(ROUND(AF10/AF5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AG12" s="10">
+      <c r="AG12" s="11">
         <f>IFERROR(ROUND(AG10/AG5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AH12" s="10">
+      <c r="AH12" s="11">
         <f>IFERROR(ROUND(AH10/AH5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AI12" s="10">
+      <c r="AI12" s="11">
         <f>IFERROR(ROUND(AI10/AI5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AJ12" s="10">
+      <c r="AJ12" s="11">
         <f>IFERROR(ROUND(AJ10/AJ5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AK12" s="10">
+      <c r="AK12" s="11">
         <f>IFERROR(ROUND(AK10/AK5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AL12" s="10">
+      <c r="AL12" s="11">
         <f>IFERROR(ROUND(AL10/AL5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AM12" s="10">
+      <c r="AM12" s="11">
         <f>IFERROR(ROUND(AM10/AM5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AN12" s="10">
+      <c r="AN12" s="11">
         <f>IFERROR(ROUND(AN10/AN5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AO12" s="10">
+      <c r="AO12" s="11">
         <f>IFERROR(ROUND(AO10/AO5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AP12" s="10">
+      <c r="AP12" s="11">
         <f>IFERROR(ROUND(AP10/AP5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AQ12" s="10">
+      <c r="AQ12" s="11">
         <f>IFERROR(ROUND(AQ10/AQ5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AR12" s="10">
+      <c r="AR12" s="11">
         <f>IFERROR(ROUND(AR10/AR5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AS12" s="10">
+      <c r="AS12" s="11">
         <f>IFERROR(ROUND(AS10/AS5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AT12" s="10">
+      <c r="AT12" s="11">
         <f>IFERROR(ROUND(AT10/AT5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AU12" s="10">
+      <c r="AU12" s="11">
         <f>IFERROR(ROUND(AU10/AU5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AV12" s="10">
+      <c r="AV12" s="11">
         <f>IFERROR(ROUND(AV10/AV5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AW12" s="10">
+      <c r="AW12" s="11">
         <f>IFERROR(ROUND(AW10/AW5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AX12" s="10">
+      <c r="AX12" s="11">
         <f>IFERROR(ROUND(AX10/AX5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AY12" s="10">
+      <c r="AY12" s="11">
         <f>IFERROR(ROUND(AY10/AY5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="AZ12" s="10">
+      <c r="AZ12" s="11">
         <f>IFERROR(ROUND(AZ10/AZ5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BA12" s="10">
+      <c r="BA12" s="11">
         <f>IFERROR(ROUND(BA10/BA5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BB12" s="10">
+      <c r="BB12" s="11">
         <f>IFERROR(ROUND(BB10/BB5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BC12" s="10">
+      <c r="BC12" s="11">
         <f>IFERROR(ROUND(BC10/BC5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BD12" s="10">
+      <c r="BD12" s="11">
         <f>IFERROR(ROUND(BD10/BD5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BE12" s="10">
+      <c r="BE12" s="11">
         <f>IFERROR(ROUND(BE10/BE5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BF12" s="10">
+      <c r="BF12" s="11">
         <f>IFERROR(ROUND(BF10/BF5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BG12" s="10">
+      <c r="BG12" s="11">
         <f>IFERROR(ROUND(BG10/BG5*100, 0), 0)</f>
         <v/>
       </c>
-      <c r="BH12" s="10">
+      <c r="BH12" s="11">
         <f>IFERROR(ROUND(BH10/BH5*100, 0), 0)</f>
-        <v/>
-      </c>
-      <c r="BI12" s="10">
-        <f>IFERROR(ROUND(BI10/BI5*100, 0), 0)</f>
         <v/>
       </c>
     </row>
     <row r="13" ht="21" customHeight="1">
-      <c r="K13" s="3">
+      <c r="K13" s="4">
         <f>MIN($P$13:$BI$13)</f>
         <v/>
       </c>
-      <c r="L13" s="4" t="n"/>
-      <c r="M13" s="3">
+      <c r="L13" s="5" t="n"/>
+      <c r="M13" s="4">
         <f>MAX($P$13:$BI$13)</f>
         <v/>
       </c>
-      <c r="O13" s="9" t="inlineStr">
+      <c r="O13" s="10" t="inlineStr">
         <is>
           <t>Budget Available</t>
         </is>
@@ -2890,13 +2872,9 @@
         <f>BH4-BH9</f>
         <v/>
       </c>
-      <c r="BI13" s="2">
-        <f>BI4-BI9</f>
-        <v/>
-      </c>
     </row>
     <row r="14" ht="21" customHeight="1">
-      <c r="O14" s="9" t="inlineStr">
+      <c r="O14" s="10" t="inlineStr">
         <is>
           <t>Brand Name</t>
         </is>
@@ -3126,10 +3104,10 @@
           <t>MAGNUM</t>
         </is>
       </c>
-      <c r="BI14" s="2" t="n"/>
+      <c r="BI14" s="3" t="n"/>
     </row>
     <row r="15" ht="21" customHeight="1">
-      <c r="O15" s="9" t="inlineStr">
+      <c r="O15" s="10" t="inlineStr">
         <is>
           <t>IB No</t>
         </is>
@@ -3359,7 +3337,7 @@
           <t>202500554425</t>
         </is>
       </c>
-      <c r="BI15" s="2" t="inlineStr">
+      <c r="BI15" s="3" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -3371,142 +3349,142 @@
           <t>Start Date</t>
         </is>
       </c>
-      <c r="P16" s="11" t="n">
+      <c r="P16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="Q16" s="11" t="n">
+      <c r="Q16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="R16" s="11" t="n">
+      <c r="R16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="S16" s="11" t="n">
+      <c r="S16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="T16" s="11" t="n">
+      <c r="T16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="U16" s="11" t="n">
+      <c r="U16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="V16" s="11" t="n">
+      <c r="V16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="W16" s="11" t="n">
+      <c r="W16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="X16" s="11" t="n">
+      <c r="X16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="Y16" s="11" t="n">
+      <c r="Y16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="Z16" s="11" t="n">
+      <c r="Z16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AA16" s="11" t="n">
+      <c r="AA16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AB16" s="11" t="n">
+      <c r="AB16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AC16" s="11" t="n">
+      <c r="AC16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AD16" s="11" t="n">
+      <c r="AD16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AE16" s="11" t="n">
+      <c r="AE16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AF16" s="11" t="n">
+      <c r="AF16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AG16" s="11" t="n">
+      <c r="AG16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AH16" s="11" t="n">
+      <c r="AH16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AI16" s="11" t="n">
+      <c r="AI16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AJ16" s="11" t="n">
+      <c r="AJ16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AK16" s="11" t="n">
+      <c r="AK16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AL16" s="11" t="n">
+      <c r="AL16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AM16" s="11" t="n">
+      <c r="AM16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AN16" s="11" t="n">
+      <c r="AN16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AO16" s="11" t="n">
+      <c r="AO16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AP16" s="11" t="n">
+      <c r="AP16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AQ16" s="11" t="n">
+      <c r="AQ16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AR16" s="11" t="n">
+      <c r="AR16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AS16" s="11" t="n">
+      <c r="AS16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AT16" s="11" t="n">
+      <c r="AT16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AU16" s="11" t="n">
+      <c r="AU16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AV16" s="11" t="n">
+      <c r="AV16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AW16" s="11" t="n">
+      <c r="AW16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AX16" s="11" t="n">
+      <c r="AX16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="AY16" s="11" t="n">
+      <c r="AY16" s="12" t="n">
         <v>45762</v>
       </c>
-      <c r="AZ16" s="11" t="n">
+      <c r="AZ16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BA16" s="11" t="n">
+      <c r="BA16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BB16" s="11" t="n">
+      <c r="BB16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BC16" s="11" t="n">
+      <c r="BC16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BD16" s="11" t="n">
+      <c r="BD16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BE16" s="11" t="n">
+      <c r="BE16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BF16" s="11" t="n">
+      <c r="BF16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BG16" s="11" t="n">
+      <c r="BG16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BH16" s="11" t="n">
+      <c r="BH16" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="BI16" s="2" t="n"/>
+      <c r="BI16" s="3" t="n"/>
     </row>
     <row r="17" ht="21" customHeight="1">
       <c r="O17" s="1" t="inlineStr">
@@ -3514,143 +3492,143 @@
           <t>End Date</t>
         </is>
       </c>
-      <c r="P17" s="11" t="n">
+      <c r="P17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="Q17" s="11" t="n">
+      <c r="Q17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="R17" s="11" t="n">
+      <c r="R17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="S17" s="11" t="n">
+      <c r="S17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="T17" s="11" t="n">
+      <c r="T17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="U17" s="11" t="n">
+      <c r="U17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="V17" s="11" t="n">
+      <c r="V17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="W17" s="11" t="n">
+      <c r="W17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="X17" s="11" t="n">
+      <c r="X17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="Y17" s="11" t="n">
+      <c r="Y17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="Z17" s="11" t="n">
+      <c r="Z17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AA17" s="11" t="n">
+      <c r="AA17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AB17" s="11" t="n">
+      <c r="AB17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AC17" s="11" t="n">
+      <c r="AC17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AD17" s="11" t="n">
+      <c r="AD17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AE17" s="11" t="n">
+      <c r="AE17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AF17" s="11" t="n">
+      <c r="AF17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AG17" s="11" t="n">
+      <c r="AG17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AH17" s="11" t="n">
+      <c r="AH17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AI17" s="11" t="n">
+      <c r="AI17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AJ17" s="11" t="n">
+      <c r="AJ17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AK17" s="11" t="n">
+      <c r="AK17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AL17" s="11" t="n">
+      <c r="AL17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AM17" s="11" t="n">
+      <c r="AM17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AN17" s="11" t="n">
+      <c r="AN17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AO17" s="11" t="n">
+      <c r="AO17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AP17" s="11" t="n">
+      <c r="AP17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AQ17" s="11" t="n">
+      <c r="AQ17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AR17" s="11" t="n">
+      <c r="AR17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AS17" s="11" t="n">
+      <c r="AS17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AT17" s="11" t="n">
+      <c r="AT17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AU17" s="11" t="n">
+      <c r="AU17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AV17" s="11" t="n">
+      <c r="AV17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AW17" s="11" t="n">
+      <c r="AW17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AX17" s="11" t="n">
+      <c r="AX17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AY17" s="11" t="n">
+      <c r="AY17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="AZ17" s="11" t="n">
+      <c r="AZ17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BA17" s="11" t="n">
+      <c r="BA17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BB17" s="11" t="n">
+      <c r="BB17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BC17" s="11" t="n">
+      <c r="BC17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BD17" s="11" t="n">
+      <c r="BD17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BE17" s="11" t="n">
+      <c r="BE17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BF17" s="11" t="n">
+      <c r="BF17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BG17" s="11" t="n">
+      <c r="BG17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BH17" s="11" t="n">
+      <c r="BH17" s="12" t="n">
         <v>45777</v>
       </c>
-      <c r="BI17" s="2" t="n"/>
-      <c r="BL17" s="5">
+      <c r="BI17" s="3" t="n"/>
+      <c r="BL17" s="6">
         <f>ROUND((BJ18/BJ5)*100, 0)</f>
         <v/>
       </c>
@@ -3841,20 +3819,16 @@
         <f>18*BH1</f>
         <v/>
       </c>
-      <c r="BI18" s="2">
-        <f>18*BI1</f>
-        <v/>
-      </c>
-      <c r="BJ18" s="9">
-        <f>SUM(BJ20:BJ9530)</f>
-        <v/>
-      </c>
-      <c r="BK18" s="9">
-        <f>SUM(BK20:BK9530)</f>
-        <v/>
-      </c>
-      <c r="BL18" s="9">
-        <f>(BK18/BJ18)*100000</f>
+      <c r="BJ18" s="10">
+        <f>SUM(BJ24:BJ55)</f>
+        <v/>
+      </c>
+      <c r="BK18" s="10">
+        <f>SUM(BK24:BK55)</f>
+        <v/>
+      </c>
+      <c r="BL18" s="10">
+        <f>IFERROR(( BK18 / BJ18 ) * 100000, 0)</f>
         <v/>
       </c>
     </row>
@@ -4044,10 +4018,6 @@
         <f>BH10-BH24</f>
         <v/>
       </c>
-      <c r="BI19" s="2">
-        <f>BI10-BI24</f>
-        <v/>
-      </c>
     </row>
     <row r="20" ht="21" customHeight="1">
       <c r="O20" s="1" t="inlineStr">
@@ -4190,7 +4160,7 @@
       <c r="BH20" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="BI20" s="2" t="n"/>
+      <c r="BI20" s="3" t="n"/>
     </row>
     <row r="21" ht="21" customHeight="1">
       <c r="O21" s="1" t="inlineStr">
@@ -4423,75 +4393,75 @@
           <t>ENG</t>
         </is>
       </c>
-      <c r="BI21" s="2" t="n"/>
+      <c r="BI21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="12" t="inlineStr">
+      <c r="B22" s="13" t="inlineStr">
         <is>
           <t>Input File F to G</t>
         </is>
       </c>
-      <c r="C22" s="12" t="inlineStr">
+      <c r="C22" s="13" t="inlineStr">
         <is>
           <t>Input File E</t>
         </is>
       </c>
-      <c r="D22" s="12" t="inlineStr">
+      <c r="D22" s="13" t="inlineStr">
         <is>
           <t>Input File A</t>
         </is>
       </c>
-      <c r="E22" s="12" t="inlineStr">
+      <c r="E22" s="13" t="inlineStr">
         <is>
           <t>Input File N</t>
         </is>
       </c>
-      <c r="F22" s="12" t="inlineStr">
+      <c r="F22" s="13" t="inlineStr">
         <is>
           <t>L/(M/N)</t>
         </is>
       </c>
-      <c r="G22" s="12" t="inlineStr">
+      <c r="G22" s="13" t="inlineStr">
         <is>
           <t>Input File E : RODP-Start</t>
         </is>
       </c>
-      <c r="H22" s="12" t="inlineStr">
+      <c r="H22" s="13" t="inlineStr">
         <is>
           <t>Input File E : RODP-End</t>
         </is>
       </c>
-      <c r="I22" s="12" t="inlineStr">
+      <c r="I22" s="13" t="inlineStr">
         <is>
           <t>hardcoded to 1</t>
         </is>
       </c>
-      <c r="J22" s="12" t="inlineStr">
+      <c r="J22" s="13" t="inlineStr">
         <is>
           <t>Day From Date</t>
         </is>
       </c>
-      <c r="K22" s="12" t="inlineStr">
+      <c r="K22" s="13" t="inlineStr">
         <is>
           <t>'='Allocated</t>
         </is>
       </c>
-      <c r="L22" s="12" t="inlineStr">
+      <c r="L22" s="13" t="inlineStr">
         <is>
           <t>sum P20 to CN20</t>
         </is>
       </c>
-      <c r="M22" s="12" t="inlineStr">
+      <c r="M22" s="13" t="inlineStr">
         <is>
           <t>sum P20*P1-CN20*CN1</t>
         </is>
       </c>
-      <c r="N22" s="12" t="inlineStr">
+      <c r="N22" s="13" t="inlineStr">
         <is>
           <t>N-M</t>
         </is>
       </c>
-      <c r="O22" s="12" t="inlineStr">
+      <c r="O22" s="13" t="inlineStr">
         <is>
           <t>Hardcoded To As Per Deal</t>
         </is>
@@ -4573,7 +4543,7 @@
           <t>PT or NPT</t>
         </is>
       </c>
-      <c r="P23" s="13" t="inlineStr">
+      <c r="P23" s="14" t="inlineStr">
         <is>
           <t>Spots</t>
         </is>
@@ -4621,8 +4591,6 @@
       <c r="BE23" s="1" t="n"/>
       <c r="BF23" s="1" t="n"/>
       <c r="BG23" s="1" t="n"/>
-      <c r="BH23" s="1" t="n"/>
-      <c r="BI23" s="1" t="n"/>
       <c r="BJ23" s="1" t="inlineStr">
         <is>
           <t>TOTAL GRP</t>
@@ -4678,13 +4646,13 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>1200</v>
+        <v>1170</v>
       </c>
       <c r="L24" t="n">
         <v>88</v>
       </c>
       <c r="M24" t="n">
-        <v>1200</v>
+        <v>1170</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -4882,13 +4850,13 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>1080</v>
+        <v>1050</v>
       </c>
       <c r="L25" t="n">
         <v>91</v>
       </c>
       <c r="M25" t="n">
-        <v>1080</v>
+        <v>1050</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -5086,13 +5054,13 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>895</v>
+        <v>865</v>
       </c>
       <c r="L26" t="n">
         <v>91</v>
       </c>
       <c r="M26" t="n">
-        <v>895</v>
+        <v>865</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -5290,13 +5258,13 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>730</v>
+        <v>700</v>
       </c>
       <c r="L27" t="n">
         <v>95</v>
       </c>
       <c r="M27" t="n">
-        <v>730</v>
+        <v>700</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -5494,13 +5462,13 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>680</v>
+        <v>650</v>
       </c>
       <c r="L28" t="n">
         <v>91</v>
       </c>
       <c r="M28" t="n">
-        <v>680</v>
+        <v>650</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -5698,13 +5666,13 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>515</v>
+        <v>485</v>
       </c>
       <c r="L29" t="n">
         <v>93</v>
       </c>
       <c r="M29" t="n">
-        <v>515</v>
+        <v>485</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>

</xml_diff>